<commit_message>
modificacion valor template caso base
</commit_message>
<xml_diff>
--- a/Capex.Web/Capex.Web/Files/Downloads/TemplateCBCD_Vacio.xlsx
+++ b/Capex.Web/Capex.Web/Files/Downloads/TemplateCBCD_Vacio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Cuevas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030A53B7-D47B-4BE1-9B55-5E6CC27B04CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B481CB8-9256-4F57-8468-C23E52232B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="6" r:id="rId1"/>
@@ -1022,7 +1022,7 @@
   <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1050,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -1089,7 +1089,7 @@
       <c r="E9" s="51"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yHpUohKIaqRekLLVMzw7ya5ujVtThwnjga/k7n6z/mpT28rxeLqG3phXFmQDWUMUpSXYTiZM8G3cPzZ3GCgqhQ==" saltValue="ht+bWuirdF9vqvlsW0/Lig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KhkWr1Cv0NLZvffaqOv+fkWAXKJ4HoisXx4wuhFT57NwUc9zZMZW2XsDtEpvXAkYFxL52UUkF0WV2PbzAIf33A==" saltValue="g5PFPWyYqUf+x94XneipUA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="B9:E9"/>
   </mergeCells>
@@ -1102,9 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CS31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="16" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,19 +1141,19 @@
       </c>
       <c r="M1" s="15">
         <f>D6</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="N1" s="15">
         <f>M1+1</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="O1" s="15">
         <f>N1+1</f>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="P1" s="15">
         <f>O1+1</f>
-        <v>2023</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="2" spans="1:97" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1174,16 +1174,16 @@
         <v>49</v>
       </c>
       <c r="M2" s="16">
-        <v>680</v>
+        <v>783</v>
       </c>
       <c r="N2" s="16">
-        <v>650</v>
+        <v>768</v>
       </c>
       <c r="O2" s="16">
-        <v>650</v>
+        <v>763</v>
       </c>
       <c r="P2" s="16">
-        <v>635</v>
+        <v>733</v>
       </c>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.25">
@@ -1204,16 +1204,16 @@
         <v>50</v>
       </c>
       <c r="M3" s="16">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="N3" s="16">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="O3" s="16">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="P3" s="16">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:97" x14ac:dyDescent="0.25">
@@ -1232,16 +1232,16 @@
         <v>51</v>
       </c>
       <c r="M4" s="16">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="N4" s="16">
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="O4" s="16">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="P4" s="16">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:97" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="D6" s="66">
         <f>General!C4</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E6" s="67"/>
       <c r="F6" s="67"/>
@@ -1290,323 +1290,323 @@
       <c r="P6" s="67"/>
       <c r="Q6" s="63">
         <f>+D6+1</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="R6" s="63">
         <f>+Q6+1</f>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="S6" s="63">
         <f t="shared" ref="S6" si="0">+R6+1</f>
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="T6" s="63">
         <f t="shared" ref="T6" si="1">+S6+1</f>
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="U6" s="63">
         <f t="shared" ref="U6" si="2">+T6+1</f>
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="V6" s="63">
         <f t="shared" ref="V6" si="3">+U6+1</f>
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="W6" s="63">
         <f t="shared" ref="W6" si="4">+V6+1</f>
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="X6" s="63">
         <f t="shared" ref="X6" si="5">+W6+1</f>
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="Y6" s="63">
         <f t="shared" ref="Y6" si="6">+X6+1</f>
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="Z6" s="63">
         <f t="shared" ref="Z6" si="7">+Y6+1</f>
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="AA6" s="63">
         <f t="shared" ref="AA6" si="8">+Z6+1</f>
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="AB6" s="63">
         <f t="shared" ref="AB6" si="9">+AA6+1</f>
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="AC6" s="63">
         <f t="shared" ref="AC6" si="10">+AB6+1</f>
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="AD6" s="63">
         <f t="shared" ref="AD6" si="11">+AC6+1</f>
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="AE6" s="63">
         <f t="shared" ref="AE6" si="12">+AD6+1</f>
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="AF6" s="63">
         <f t="shared" ref="AF6" si="13">+AE6+1</f>
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="AG6" s="63">
         <f t="shared" ref="AG6" si="14">+AF6+1</f>
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="AH6" s="63">
         <f t="shared" ref="AH6" si="15">+AG6+1</f>
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="AI6" s="63">
         <f t="shared" ref="AI6" si="16">+AH6+1</f>
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="AJ6" s="63">
         <f t="shared" ref="AJ6" si="17">+AI6+1</f>
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="AK6" s="63">
         <f t="shared" ref="AK6" si="18">+AJ6+1</f>
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="AL6" s="63">
         <f t="shared" ref="AL6" si="19">+AK6+1</f>
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="AM6" s="63">
         <f t="shared" ref="AM6" si="20">+AL6+1</f>
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="AN6" s="63">
         <f t="shared" ref="AN6" si="21">+AM6+1</f>
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="AO6" s="63">
         <f t="shared" ref="AO6" si="22">+AN6+1</f>
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AP6" s="63">
         <f t="shared" ref="AP6" si="23">+AO6+1</f>
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AQ6" s="63">
         <f t="shared" ref="AQ6" si="24">+AP6+1</f>
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AR6" s="63">
         <f t="shared" ref="AR6" si="25">+AQ6+1</f>
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AS6" s="63">
         <f t="shared" ref="AS6" si="26">+AR6+1</f>
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="AT6" s="63">
         <f t="shared" ref="AT6" si="27">+AS6+1</f>
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="AU6" s="63">
         <f t="shared" ref="AU6" si="28">+AT6+1</f>
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="AV6" s="63">
         <f t="shared" ref="AV6" si="29">+AU6+1</f>
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="AW6" s="63">
         <f t="shared" ref="AW6" si="30">+AV6+1</f>
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="AX6" s="63">
         <f t="shared" ref="AX6" si="31">+AW6+1</f>
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="AY6" s="63">
         <f t="shared" ref="AY6" si="32">+AX6+1</f>
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="AZ6" s="63">
         <f t="shared" ref="AZ6" si="33">+AY6+1</f>
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="BA6" s="63">
         <f t="shared" ref="BA6" si="34">+AZ6+1</f>
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="BB6" s="63">
         <f t="shared" ref="BB6" si="35">+BA6+1</f>
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="BC6" s="63">
         <f t="shared" ref="BC6" si="36">+BB6+1</f>
-        <v>2059</v>
+        <v>2060</v>
       </c>
       <c r="BD6" s="63">
         <f t="shared" ref="BD6" si="37">+BC6+1</f>
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="BE6" s="63">
         <f t="shared" ref="BE6" si="38">+BD6+1</f>
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="BF6" s="63">
         <f t="shared" ref="BF6" si="39">+BE6+1</f>
-        <v>2062</v>
+        <v>2063</v>
       </c>
       <c r="BG6" s="63">
         <f t="shared" ref="BG6" si="40">+BF6+1</f>
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="BH6" s="63">
         <f t="shared" ref="BH6" si="41">+BG6+1</f>
-        <v>2064</v>
+        <v>2065</v>
       </c>
       <c r="BI6" s="63">
         <f t="shared" ref="BI6" si="42">+BH6+1</f>
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="BJ6" s="63">
         <f t="shared" ref="BJ6" si="43">+BI6+1</f>
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="BK6" s="63">
         <f t="shared" ref="BK6" si="44">+BJ6+1</f>
-        <v>2067</v>
+        <v>2068</v>
       </c>
       <c r="BL6" s="63">
         <f t="shared" ref="BL6" si="45">+BK6+1</f>
-        <v>2068</v>
+        <v>2069</v>
       </c>
       <c r="BM6" s="63">
         <f t="shared" ref="BM6" si="46">+BL6+1</f>
-        <v>2069</v>
+        <v>2070</v>
       </c>
       <c r="BN6" s="63">
         <f t="shared" ref="BN6" si="47">+BM6+1</f>
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="BO6" s="63">
         <f t="shared" ref="BO6" si="48">+BN6+1</f>
-        <v>2071</v>
+        <v>2072</v>
       </c>
       <c r="BP6" s="63">
         <f t="shared" ref="BP6" si="49">+BO6+1</f>
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="BQ6" s="63">
         <f t="shared" ref="BQ6" si="50">+BP6+1</f>
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="BR6" s="63">
         <f t="shared" ref="BR6" si="51">+BQ6+1</f>
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="BS6" s="63">
         <f t="shared" ref="BS6" si="52">+BR6+1</f>
-        <v>2075</v>
+        <v>2076</v>
       </c>
       <c r="BT6" s="63">
         <f t="shared" ref="BT6" si="53">+BS6+1</f>
-        <v>2076</v>
+        <v>2077</v>
       </c>
       <c r="BU6" s="63">
         <f t="shared" ref="BU6" si="54">+BT6+1</f>
-        <v>2077</v>
+        <v>2078</v>
       </c>
       <c r="BV6" s="63">
         <f t="shared" ref="BV6" si="55">+BU6+1</f>
-        <v>2078</v>
+        <v>2079</v>
       </c>
       <c r="BW6" s="63">
         <f t="shared" ref="BW6" si="56">+BV6+1</f>
-        <v>2079</v>
+        <v>2080</v>
       </c>
       <c r="BX6" s="63">
         <f t="shared" ref="BX6" si="57">+BW6+1</f>
-        <v>2080</v>
+        <v>2081</v>
       </c>
       <c r="BY6" s="63">
         <f t="shared" ref="BY6" si="58">+BX6+1</f>
-        <v>2081</v>
+        <v>2082</v>
       </c>
       <c r="BZ6" s="63">
         <f t="shared" ref="BZ6" si="59">+BY6+1</f>
-        <v>2082</v>
+        <v>2083</v>
       </c>
       <c r="CA6" s="63">
         <f t="shared" ref="CA6" si="60">+BZ6+1</f>
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="CB6" s="63">
         <f t="shared" ref="CB6" si="61">+CA6+1</f>
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="CC6" s="63">
         <f t="shared" ref="CC6" si="62">+CB6+1</f>
-        <v>2085</v>
+        <v>2086</v>
       </c>
       <c r="CD6" s="63">
         <f t="shared" ref="CD6" si="63">+CC6+1</f>
-        <v>2086</v>
+        <v>2087</v>
       </c>
       <c r="CE6" s="63">
         <f t="shared" ref="CE6" si="64">+CD6+1</f>
-        <v>2087</v>
+        <v>2088</v>
       </c>
       <c r="CF6" s="63">
         <f t="shared" ref="CF6" si="65">+CE6+1</f>
-        <v>2088</v>
+        <v>2089</v>
       </c>
       <c r="CG6" s="63">
         <f t="shared" ref="CG6" si="66">+CF6+1</f>
-        <v>2089</v>
+        <v>2090</v>
       </c>
       <c r="CH6" s="63">
         <f t="shared" ref="CH6" si="67">+CG6+1</f>
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="CI6" s="63">
         <f t="shared" ref="CI6" si="68">+CH6+1</f>
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="CJ6" s="63">
         <f t="shared" ref="CJ6" si="69">+CI6+1</f>
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="CK6" s="63">
         <f t="shared" ref="CK6" si="70">+CJ6+1</f>
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="CL6" s="63">
         <f t="shared" ref="CL6" si="71">+CK6+1</f>
-        <v>2094</v>
+        <v>2095</v>
       </c>
       <c r="CM6" s="63">
         <f t="shared" ref="CM6" si="72">+CL6+1</f>
-        <v>2095</v>
+        <v>2096</v>
       </c>
       <c r="CN6" s="63">
         <f t="shared" ref="CN6" si="73">+CM6+1</f>
-        <v>2096</v>
+        <v>2097</v>
       </c>
       <c r="CO6" s="63">
         <f t="shared" ref="CO6" si="74">+CN6+1</f>
-        <v>2097</v>
+        <v>2098</v>
       </c>
       <c r="CP6" s="63">
         <f t="shared" ref="CP6" si="75">+CO6+1</f>
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="CQ6" s="63">
         <f t="shared" ref="CQ6" si="76">+CP6+1</f>
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="CR6" s="63">
         <f t="shared" ref="CR6" si="77">+CQ6+1</f>
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="CS6" s="63" t="s">
         <v>20</v>
@@ -8278,7 +8278,7 @@
       </c>
       <c r="B29" s="24">
         <f>General!C4</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>20</v>
@@ -8336,7 +8336,7 @@
       <c r="H31" s="13"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Jt1uhGuqOWvzjyli5wYz4wJJU0IH8sfQ0yODpVw3YWpWZ3jiHZ1Ml9+k3jwQrSu1nS850lqguhEljhAvjomkGA==" saltValue="oBMj7qPWKi5C8zOW2XXvwQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nGwhZshFJGzg5N8+Hw8zG+EfcvKfahwMWdZtWkYb51RIXOD/uCa+9D77YystJfKmfACj1obg+HbrPP8yvi69VA==" saltValue="WHuiDhiyoLPH+GHhIjxhpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="100">
     <mergeCell ref="CN6:CN7"/>
     <mergeCell ref="CO6:CO7"/>
@@ -8448,7 +8448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:CT12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="16" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -8519,7 +8519,7 @@
       </c>
       <c r="D3" s="71">
         <f>General!C4</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E3" s="72"/>
       <c r="F3" s="72"/>
@@ -8535,323 +8535,323 @@
       <c r="P3" s="73"/>
       <c r="Q3" s="63">
         <f>+D3+1</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="R3" s="63">
         <f>+Q3+1</f>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="S3" s="63">
         <f>+R3+1</f>
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="T3" s="63">
         <f t="shared" ref="T3:AM3" si="0">+S3+1</f>
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="U3" s="63">
         <f t="shared" si="0"/>
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="V3" s="63">
         <f t="shared" si="0"/>
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="W3" s="63">
         <f t="shared" si="0"/>
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="X3" s="63">
         <f t="shared" si="0"/>
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="Y3" s="63">
         <f t="shared" si="0"/>
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="Z3" s="63">
         <f t="shared" si="0"/>
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="AA3" s="63">
         <f t="shared" si="0"/>
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="AB3" s="63">
         <f t="shared" si="0"/>
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="AC3" s="63">
         <f t="shared" si="0"/>
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="AD3" s="63">
         <f t="shared" si="0"/>
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="AE3" s="63">
         <f t="shared" si="0"/>
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="AF3" s="63">
         <f t="shared" si="0"/>
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="AG3" s="63">
         <f t="shared" si="0"/>
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="AH3" s="63">
         <f t="shared" si="0"/>
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="AI3" s="63">
         <f t="shared" si="0"/>
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="AJ3" s="63">
         <f t="shared" si="0"/>
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="AK3" s="63">
         <f t="shared" si="0"/>
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="AL3" s="63">
         <f t="shared" si="0"/>
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="AM3" s="63">
         <f t="shared" si="0"/>
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="AN3" s="63">
         <f t="shared" ref="AN3:BJ3" si="1">+AM3+1</f>
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="AO3" s="63">
         <f t="shared" si="1"/>
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AP3" s="63">
         <f t="shared" si="1"/>
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AQ3" s="63">
         <f t="shared" si="1"/>
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AR3" s="63">
         <f t="shared" si="1"/>
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AS3" s="63">
         <f t="shared" si="1"/>
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="AT3" s="63">
         <f t="shared" si="1"/>
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="AU3" s="63">
         <f t="shared" si="1"/>
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="AV3" s="63">
         <f t="shared" si="1"/>
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="AW3" s="63">
         <f t="shared" si="1"/>
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="AX3" s="63">
         <f t="shared" si="1"/>
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="AY3" s="63">
         <f t="shared" si="1"/>
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="AZ3" s="63">
         <f t="shared" si="1"/>
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="BA3" s="63">
         <f t="shared" si="1"/>
-        <v>2057</v>
+        <v>2058</v>
       </c>
       <c r="BB3" s="63">
         <f t="shared" si="1"/>
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="BC3" s="63">
         <f t="shared" si="1"/>
-        <v>2059</v>
+        <v>2060</v>
       </c>
       <c r="BD3" s="63">
         <f t="shared" si="1"/>
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="BE3" s="63">
         <f t="shared" si="1"/>
-        <v>2061</v>
+        <v>2062</v>
       </c>
       <c r="BF3" s="63">
         <f t="shared" si="1"/>
-        <v>2062</v>
+        <v>2063</v>
       </c>
       <c r="BG3" s="63">
         <f t="shared" si="1"/>
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="BH3" s="63">
         <f t="shared" si="1"/>
-        <v>2064</v>
+        <v>2065</v>
       </c>
       <c r="BI3" s="63">
         <f t="shared" si="1"/>
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="BJ3" s="63">
         <f t="shared" si="1"/>
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="BK3" s="63">
         <f t="shared" ref="BK3:BM3" si="2">+BJ3+1</f>
-        <v>2067</v>
+        <v>2068</v>
       </c>
       <c r="BL3" s="63">
         <f t="shared" si="2"/>
-        <v>2068</v>
+        <v>2069</v>
       </c>
       <c r="BM3" s="63">
         <f t="shared" si="2"/>
-        <v>2069</v>
+        <v>2070</v>
       </c>
       <c r="BN3" s="63">
         <f t="shared" ref="BN3:CP3" si="3">+BM3+1</f>
-        <v>2070</v>
+        <v>2071</v>
       </c>
       <c r="BO3" s="63">
         <f t="shared" si="3"/>
-        <v>2071</v>
+        <v>2072</v>
       </c>
       <c r="BP3" s="63">
         <f t="shared" si="3"/>
-        <v>2072</v>
+        <v>2073</v>
       </c>
       <c r="BQ3" s="63">
         <f t="shared" si="3"/>
-        <v>2073</v>
+        <v>2074</v>
       </c>
       <c r="BR3" s="63">
         <f t="shared" si="3"/>
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="BS3" s="63">
         <f t="shared" si="3"/>
-        <v>2075</v>
+        <v>2076</v>
       </c>
       <c r="BT3" s="63">
         <f t="shared" si="3"/>
-        <v>2076</v>
+        <v>2077</v>
       </c>
       <c r="BU3" s="63">
         <f t="shared" si="3"/>
-        <v>2077</v>
+        <v>2078</v>
       </c>
       <c r="BV3" s="63">
         <f t="shared" si="3"/>
-        <v>2078</v>
+        <v>2079</v>
       </c>
       <c r="BW3" s="63">
         <f t="shared" si="3"/>
-        <v>2079</v>
+        <v>2080</v>
       </c>
       <c r="BX3" s="63">
         <f t="shared" si="3"/>
-        <v>2080</v>
+        <v>2081</v>
       </c>
       <c r="BY3" s="63">
         <f t="shared" si="3"/>
-        <v>2081</v>
+        <v>2082</v>
       </c>
       <c r="BZ3" s="63">
         <f t="shared" si="3"/>
-        <v>2082</v>
+        <v>2083</v>
       </c>
       <c r="CA3" s="63">
         <f t="shared" si="3"/>
-        <v>2083</v>
+        <v>2084</v>
       </c>
       <c r="CB3" s="63">
         <f t="shared" si="3"/>
-        <v>2084</v>
+        <v>2085</v>
       </c>
       <c r="CC3" s="63">
         <f t="shared" si="3"/>
-        <v>2085</v>
+        <v>2086</v>
       </c>
       <c r="CD3" s="63">
         <f t="shared" si="3"/>
-        <v>2086</v>
+        <v>2087</v>
       </c>
       <c r="CE3" s="63">
         <f t="shared" si="3"/>
-        <v>2087</v>
+        <v>2088</v>
       </c>
       <c r="CF3" s="63">
         <f t="shared" si="3"/>
-        <v>2088</v>
+        <v>2089</v>
       </c>
       <c r="CG3" s="63">
         <f t="shared" si="3"/>
-        <v>2089</v>
+        <v>2090</v>
       </c>
       <c r="CH3" s="63">
         <f t="shared" si="3"/>
-        <v>2090</v>
+        <v>2091</v>
       </c>
       <c r="CI3" s="63">
         <f t="shared" si="3"/>
-        <v>2091</v>
+        <v>2092</v>
       </c>
       <c r="CJ3" s="63">
         <f t="shared" si="3"/>
-        <v>2092</v>
+        <v>2093</v>
       </c>
       <c r="CK3" s="63">
         <f t="shared" si="3"/>
-        <v>2093</v>
+        <v>2094</v>
       </c>
       <c r="CL3" s="63">
         <f t="shared" si="3"/>
-        <v>2094</v>
+        <v>2095</v>
       </c>
       <c r="CM3" s="63">
         <f t="shared" si="3"/>
-        <v>2095</v>
+        <v>2096</v>
       </c>
       <c r="CN3" s="63">
         <f t="shared" si="3"/>
-        <v>2096</v>
+        <v>2097</v>
       </c>
       <c r="CO3" s="63">
         <f t="shared" si="3"/>
-        <v>2097</v>
+        <v>2098</v>
       </c>
       <c r="CP3" s="63">
         <f t="shared" si="3"/>
-        <v>2098</v>
+        <v>2099</v>
       </c>
       <c r="CQ3" s="63">
         <f t="shared" ref="CQ3:CR3" si="4">+CP3+1</f>
-        <v>2099</v>
+        <v>2100</v>
       </c>
       <c r="CR3" s="63">
         <f t="shared" si="4"/>
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="CS3" s="63" t="s">
         <v>34</v>

</xml_diff>